<commit_message>
[reorder] folders, duplicated electrics schemes and flowdiagrams
</commit_message>
<xml_diff>
--- a/Documenten/Productbacklog/productbacklog.xlsx
+++ b/Documenten/Productbacklog/productbacklog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hrnl-my.sharepoint.com/personal/0987057_hr_nl/Documents/2021 Technische informatica 2/Project-5-6/Documenten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hrnl-my.sharepoint.com/personal/0987057_hr_nl/Documents/2021 Technische informatica 2/Project-5-6/Documenten/Productbacklog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="379" documentId="8_{C8EFED4C-861F-4D9A-A52C-382DCF3D3507}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD2A7EF1-F555-44DC-B5F1-7E89F6C9D2B8}"/>
+  <xr:revisionPtr revIDLastSave="384" documentId="8_{C8EFED4C-861F-4D9A-A52C-382DCF3D3507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FC3B030-F47C-4A5F-A055-8061FAF348F3}"/>
   <bookViews>
     <workbookView xWindow="4965" yWindow="16080" windowWidth="29040" windowHeight="16440" xr2:uid="{AB4C6EDC-C71E-401F-AB46-2C9C4233DE0F}"/>
   </bookViews>
@@ -219,7 +219,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,13 +230,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -262,7 +255,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,18 +277,6 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -306,15 +287,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -328,10 +307,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -340,37 +319,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="5" builtinId="52"/>
+  <cellStyles count="4">
     <cellStyle name="Goed" xfId="3" builtinId="26"/>
     <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
     <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
@@ -689,7 +654,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,19 +713,19 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -806,7 +771,7 @@
       <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>49</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -827,7 +792,7 @@
       <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>51</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -848,7 +813,7 @@
       <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -859,19 +824,19 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="11">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" t="s">
         <v>35</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -892,7 +857,7 @@
       <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -934,7 +899,7 @@
       <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -942,14 +907,14 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">

</xml_diff>